<commit_message>
Re-drafted introduction, started method. Also did some source code rearranging and making figures
</commit_message>
<xml_diff>
--- a/Writing/table2.xlsx
+++ b/Writing/table2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\SkyDrive\Masterproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Dropbox\CJM\Masterproject\Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="e">
-        <f t="shared" ref="F3:F10" si="0">D3/(E3+D3)</f>
+        <f t="shared" ref="F3:F37" si="0">D3/(E3+D3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -603,7 +603,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="1" t="e">
+      <c r="F10" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -614,6 +614,22 @@
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <f>SUM(C12:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <f>SUM(D12:D19)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f>SUM(E12:E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,42 +637,70 @@
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F12" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F13" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F14" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F15" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F16" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F17" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F18" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -666,7 +710,10 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -674,6 +721,22 @@
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(C21:C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <f>SUM(D21:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(E21:E28)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,42 +744,70 @@
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F21" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F22" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F23" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F24" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F25" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F26" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F27" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -726,7 +817,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -735,54 +829,170 @@
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="C29" s="5">
+        <f>SUM(C20+C11+C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <f>SUM(D2+D11+D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <f>SUM(E20+E11+E2)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="C30" s="5">
+        <f t="shared" ref="C30:C37" si="1">SUM(C21+C12+C3)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" ref="D30:D37" si="2">SUM(D3+D12+D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" ref="E30:E37" si="3">SUM(E21+E12+E3)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="C31" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C32" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C33" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C34" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C35" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="C36" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -790,10 +1000,22 @@
       <c r="B37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="C37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>